<commit_message>
Cambios finales previo a revisión con JANS de los diccionarios
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_02.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_02.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angleito\Documents\Consultorías\wcs\04_Entregable 2\previo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="95">
   <si>
     <t>Elemento</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Identificador asignado al juicio</t>
   </si>
   <si>
-    <t>Código alfanumérico de entre 14 y 15 caractéres</t>
-  </si>
-  <si>
     <t>24281201901783</t>
   </si>
   <si>
@@ -309,6 +306,15 @@
   </si>
   <si>
     <t>RAZON DE EJECUTORIA</t>
+  </si>
+  <si>
+    <t>Evento</t>
+  </si>
+  <si>
+    <t>PROVINCIA, CANTON</t>
+  </si>
+  <si>
+    <t>Las variables de identificación deben cumplir con una extensión y combinación de caracteres específicos</t>
   </si>
 </sst>
 </file>
@@ -332,7 +338,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +348,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -399,6 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -760,64 +773,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -825,7 +838,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -837,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +908,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -903,25 +916,26 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
       <c r="C3" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -929,11 +943,12 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
+      <c r="F3" s="13"/>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I3" s="9">
         <v>43742</v>
@@ -941,129 +956,138 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
       <c r="C4" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="H7" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" t="s">
-        <v>40</v>
-      </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
       <c r="C8" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="10"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1087,64 +1111,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -1152,7 +1176,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1165,7 +1189,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G6" sqref="G6:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1246,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1230,25 +1254,26 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
       <c r="C3" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -1256,11 +1281,12 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
+      <c r="F3" s="13"/>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I3" s="9">
         <v>43754</v>
@@ -1268,181 +1294,198 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
       <c r="C4" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="H7" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" t="s">
-        <v>40</v>
-      </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
       <c r="C8" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="10"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
         <v>77</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>80</v>
-      </c>
-      <c r="J9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
         <v>82</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>84</v>
-      </c>
       <c r="H10" s="12" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="I10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" t="s">
         <v>80</v>
-      </c>
-      <c r="J10" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1466,64 +1509,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -1531,7 +1574,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1544,7 +1587,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1644,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1609,152 +1652,162 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
       <c r="C3" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
         <v>33</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="10"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="H6" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
       <c r="C7" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1762,11 +1815,12 @@
       <c r="E8" t="s">
         <v>21</v>
       </c>
+      <c r="F8" s="13"/>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" s="9">
         <v>44083</v>
@@ -1774,26 +1828,27 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
       <c r="G9" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AG: diccionarios entrega version 1.0
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_02.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_02.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angleito\Documents\Consultorías\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\04_Entregable 2\previo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="85">
   <si>
     <t>Elemento</t>
   </si>
@@ -80,12 +80,6 @@
     <t>Fuente de Datos</t>
   </si>
   <si>
-    <t>Relaciones</t>
-  </si>
-  <si>
-    <t>Reglas de Calidad</t>
-  </si>
-  <si>
     <t>Clasificación</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>No aplica</t>
   </si>
   <si>
-    <t>No debe estar vacío</t>
-  </si>
-  <si>
     <t>IDJUICIO</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
     <t>RESUELTA</t>
   </si>
   <si>
-    <t>Debe ser un cantón de la provincia asignada</t>
-  </si>
-  <si>
     <t>División político administrativa</t>
   </si>
   <si>
@@ -218,12 +206,6 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>Fechas en formato dd/mm/aaaa comprendidas entre 01/01/2019 hasta 31/08/2024</t>
-  </si>
-  <si>
-    <t>VALORES DIFERENTES A LOS PRESENTES EN LA BASE</t>
-  </si>
-  <si>
     <t>Cadena</t>
   </si>
   <si>
@@ -242,9 +224,6 @@
     <t>Localización</t>
   </si>
   <si>
-    <t>Transacción o Evento</t>
-  </si>
-  <si>
     <t>Causas Resueltas</t>
   </si>
   <si>
@@ -266,9 +245,6 @@
     <t>Resolución del juicio</t>
   </si>
   <si>
-    <t>Expresión que describe la resolución del juicio</t>
-  </si>
-  <si>
     <t>SENTENCIA CONDENATORIA</t>
   </si>
   <si>
@@ -281,9 +257,6 @@
     <t>Forma de terminación del juicio</t>
   </si>
   <si>
-    <t>Expresión que describe la forma de terminación del juicio</t>
-  </si>
-  <si>
     <t>CAUSAS RESUELTAS , "RAZON DE EJECUTORIA"</t>
   </si>
   <si>
@@ -308,13 +281,10 @@
     <t>RAZON DE EJECUTORIA</t>
   </si>
   <si>
-    <t>Evento</t>
-  </si>
-  <si>
-    <t>PROVINCIA, CANTON</t>
-  </si>
-  <si>
-    <t>Las variables de identificación deben cumplir con una extensión y combinación de caracteres específicos</t>
+    <t>Clasificación interna Judicatura</t>
+  </si>
+  <si>
+    <t>¿PUEDEN HABER VALORES DIFERENTES A LOS PRESENTES EN LA BASE?</t>
   </si>
 </sst>
 </file>
@@ -338,24 +308,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -385,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -408,10 +366,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,7 +719,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,64 +729,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -838,7 +794,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -848,34 +804,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -884,210 +838,184 @@
       <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="C3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="9">
+        <v>43742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="9">
-        <v>43742</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="C5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="C6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="H6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="12" t="s">
+      <c r="C7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I6" t="s">
+      <c r="G7" t="s">
         <v>36</v>
       </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="C8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" t="s">
-        <v>63</v>
+      <c r="H8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1111,64 +1039,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -1176,7 +1104,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1186,34 +1114,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1222,270 +1148,236 @@
       <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
       <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>64</v>
+        <v>21</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="9">
+        <v>43754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="9">
-        <v>43754</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="12" t="s">
+      <c r="C10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="13"/>
       <c r="G10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I10" t="s">
-        <v>79</v>
-      </c>
-      <c r="J10" t="s">
-        <v>80</v>
+        <v>71</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1509,64 +1401,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -1574,7 +1466,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1584,34 +1476,32 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1620,235 +1510,207 @@
       <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
       <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>64</v>
+        <v>21</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="C4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="C5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="12" t="s">
+      <c r="C6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I5" t="s">
+      <c r="G6" t="s">
         <v>36</v>
       </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="H6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="C7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="12" t="s">
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="9">
+        <v>44083</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="9">
-        <v>44083</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="13"/>
       <c r="G9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AG: preparación carpeta envío
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_02.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_02.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angleito\Documents\Consultorías\wcs\04_Entregable 2\previo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="95">
   <si>
     <t>Elemento</t>
   </si>
@@ -80,6 +80,12 @@
     <t>Fuente de Datos</t>
   </si>
   <si>
+    <t>Relaciones</t>
+  </si>
+  <si>
+    <t>Reglas de Calidad</t>
+  </si>
+  <si>
     <t>Clasificación</t>
   </si>
   <si>
@@ -92,6 +98,9 @@
     <t>No aplica</t>
   </si>
   <si>
+    <t>No debe estar vacío</t>
+  </si>
+  <si>
     <t>IDJUICIO</t>
   </si>
   <si>
@@ -152,6 +161,9 @@
     <t>RESUELTA</t>
   </si>
   <si>
+    <t>Debe ser un cantón de la provincia asignada</t>
+  </si>
+  <si>
     <t>División político administrativa</t>
   </si>
   <si>
@@ -206,6 +218,12 @@
     <t>Fecha</t>
   </si>
   <si>
+    <t>Fechas en formato dd/mm/aaaa comprendidas entre 01/01/2019 hasta 31/08/2024</t>
+  </si>
+  <si>
+    <t>VALORES DIFERENTES A LOS PRESENTES EN LA BASE</t>
+  </si>
+  <si>
     <t>Cadena</t>
   </si>
   <si>
@@ -224,6 +242,9 @@
     <t>Localización</t>
   </si>
   <si>
+    <t>Transacción o Evento</t>
+  </si>
+  <si>
     <t>Causas Resueltas</t>
   </si>
   <si>
@@ -245,6 +266,9 @@
     <t>Resolución del juicio</t>
   </si>
   <si>
+    <t>Expresión que describe la resolución del juicio</t>
+  </si>
+  <si>
     <t>SENTENCIA CONDENATORIA</t>
   </si>
   <si>
@@ -257,6 +281,9 @@
     <t>Forma de terminación del juicio</t>
   </si>
   <si>
+    <t>Expresión que describe la forma de terminación del juicio</t>
+  </si>
+  <si>
     <t>CAUSAS RESUELTAS , "RAZON DE EJECUTORIA"</t>
   </si>
   <si>
@@ -281,10 +308,13 @@
     <t>RAZON DE EJECUTORIA</t>
   </si>
   <si>
-    <t>Clasificación interna Judicatura</t>
-  </si>
-  <si>
-    <t>¿PUEDEN HABER VALORES DIFERENTES A LOS PRESENTES EN LA BASE?</t>
+    <t>Evento</t>
+  </si>
+  <si>
+    <t>PROVINCIA, CANTON</t>
+  </si>
+  <si>
+    <t>Las variables de identificación deben cumplir con una extensión y combinación de caracteres específicos</t>
   </si>
 </sst>
 </file>
@@ -308,12 +338,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -343,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -366,8 +408,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,7 +763,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,64 +773,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -794,7 +838,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -804,32 +848,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -838,184 +884,210 @@
       <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>58</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="9">
+        <v>43742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="9">
-        <v>43742</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="H4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
         <v>63</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1039,64 +1111,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -1104,7 +1176,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1114,32 +1186,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G6" sqref="G6:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1148,236 +1222,270 @@
       <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>58</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="9">
+        <v>43754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="9">
-        <v>43754</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="H4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
         <v>63</v>
       </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" t="s">
-        <v>72</v>
+      <c r="H10" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1401,64 +1509,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B7" s="9">
         <v>45535</v>
@@ -1466,7 +1574,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1476,32 +1584,34 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1510,207 +1620,235 @@
       <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>58</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="H3" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" t="s">
         <v>63</v>
       </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>59</v>
+        <v>89</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="9">
+      <c r="H8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="9">
         <v>44083</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>6</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>22</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>